<commit_message>
chnages to test case
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="69">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -224,13 +224,31 @@
   </si>
   <si>
     <t>US/CA (+1)</t>
+  </si>
+  <si>
+    <t>MID</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Standalone Refund</t>
+  </si>
+  <si>
+    <t>TransactionCardType</t>
+  </si>
+  <si>
+    <t>CreditCard</t>
+  </si>
+  <si>
+    <t>6280888815760052</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +270,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF313131"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -275,12 +299,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -596,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB8"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,9 +638,11 @@
     <col min="19" max="19" width="13.90625" customWidth="1"/>
     <col min="20" max="20" width="13" customWidth="1"/>
     <col min="21" max="21" width="11.54296875" customWidth="1"/>
+    <col min="29" max="29" width="21" customWidth="1"/>
+    <col min="31" max="31" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -700,8 +727,17 @@
       <c r="AB1" t="s">
         <v>61</v>
       </c>
+      <c r="AC1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -769,7 +805,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -833,8 +869,17 @@
       <c r="AA3" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="AC3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -899,7 +944,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -964,7 +1009,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1029,7 +1074,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1094,7 +1139,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1173,5 +1218,6 @@
     <hyperlink ref="H8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to test cases
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deluxe\Deluxe_UiPathProject\Deluxe_TestAutomationProject\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deluxe\Deluxe_UiPathProject\Deluxe_TestAutomationProject\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="183">
   <si>
     <t>Module</t>
   </si>
@@ -60,204 +60,249 @@
     <t>CreatePayment_Token</t>
   </si>
   <si>
+    <t>API_TestCases\CreateSubscription_Card.xaml</t>
+  </si>
+  <si>
+    <t>CreateSubscription_Card</t>
+  </si>
+  <si>
+    <t>Payments_NewCustomer</t>
+  </si>
+  <si>
+    <t>Payments\PaymentsNewCustomer\TC_11055 and TC_11056.xaml</t>
+  </si>
+  <si>
+    <t>TC_11055 and TC_11056</t>
+  </si>
+  <si>
+    <t>Payments\PaymentsNewCustomer\TC_11057 and TC_11058.xaml</t>
+  </si>
+  <si>
+    <t>TC_11057 and TC_11058</t>
+  </si>
+  <si>
+    <t>Payments\PaymentsNewCustomer\TC_11059 and TC_11060.xaml</t>
+  </si>
+  <si>
+    <t>TC_11059 and TC_11060</t>
+  </si>
+  <si>
+    <t>Payments\PaymentsNewCustomer\TC_11061 and TC_11062.xaml</t>
+  </si>
+  <si>
+    <t>TC_11061 and TC_11062</t>
+  </si>
+  <si>
+    <t>Payments\PaymentsNewCustomer\TC_11063 and TC_11064.xaml</t>
+  </si>
+  <si>
+    <t>TC_11063 and TC_11064</t>
+  </si>
+  <si>
     <t>Payments_VaultCustomer</t>
   </si>
   <si>
-    <t>Payments\Payments_VaultCustomer\TC_11075.xaml</t>
-  </si>
-  <si>
-    <t>TC_11075</t>
-  </si>
-  <si>
-    <t>Payments\Payments_VaultCustomer\TC_11076.xaml</t>
-  </si>
-  <si>
-    <t>TC_11076</t>
-  </si>
-  <si>
-    <t>API_TestCases\CreateSubscription_Card.xaml</t>
-  </si>
-  <si>
-    <t>CreateSubscription_Card</t>
-  </si>
-  <si>
-    <t>Payments_NewCustomer</t>
-  </si>
-  <si>
-    <t>Payments\PaymentsNewCustomer\TC_11057.xaml</t>
+    <t>Payments\Payments_VaultCustomer\TC_11067 and TC_11068.xaml</t>
+  </si>
+  <si>
+    <t>TC_11067 and TC_11068</t>
+  </si>
+  <si>
+    <t>Payments\Payments_VaultCustomer\TC_11069 and TC_11070.xaml</t>
+  </si>
+  <si>
+    <t>TC_11069 and TC_11070</t>
+  </si>
+  <si>
+    <t>Payments\Payments_VaultCustomer\TC_11071 and TC_11072.xaml</t>
+  </si>
+  <si>
+    <t>TC_11071 and TC_11072</t>
+  </si>
+  <si>
+    <t>Payments\Payments_VaultCustomer\TC_11073 and TC_11074.xaml</t>
+  </si>
+  <si>
+    <t>TC_11073 and TC_11074</t>
+  </si>
+  <si>
+    <t>Payments\Payments_VaultCustomer\TC_11075 and TC_11076.xaml</t>
+  </si>
+  <si>
+    <t>TC_11075 and TC_11076</t>
+  </si>
+  <si>
+    <t>TestCaseId</t>
+  </si>
+  <si>
+    <t>PaymentMethod</t>
+  </si>
+  <si>
+    <t>MerchantName</t>
+  </si>
+  <si>
+    <t>VaultCustomerName</t>
+  </si>
+  <si>
+    <t>TotalAmount</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>PaymentType</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>CardExpiry</t>
+  </si>
+  <si>
+    <t>CardType</t>
+  </si>
+  <si>
+    <t>QuickSaleItemName</t>
+  </si>
+  <si>
+    <t>QuickSaleItemPrice</t>
+  </si>
+  <si>
+    <t>QuickSaleItemTax</t>
+  </si>
+  <si>
+    <t>PresetSaleItem</t>
+  </si>
+  <si>
+    <t>CustomerAddress</t>
+  </si>
+  <si>
+    <t>CustomerState</t>
+  </si>
+  <si>
+    <t>CustomerCity</t>
+  </si>
+  <si>
+    <t>CustomerZipCode</t>
+  </si>
+  <si>
+    <t>CustomerCountry</t>
+  </si>
+  <si>
+    <t>CountryCode</t>
+  </si>
+  <si>
+    <t>OrderNote</t>
+  </si>
+  <si>
+    <t>DiscountRate</t>
+  </si>
+  <si>
+    <t>TaxAmount</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>PhoneCode</t>
+  </si>
+  <si>
+    <t>MID</t>
+  </si>
+  <si>
+    <t>TransactionCardType</t>
+  </si>
+  <si>
+    <t>FaxNumber</t>
+  </si>
+  <si>
+    <t>TC_11001</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>QA Fee Test</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>5555555555554444</t>
+  </si>
+  <si>
+    <t>mastercard</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>No Tax</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Buy Fruits</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>TC_11055</t>
+  </si>
+  <si>
+    <t>Refund</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>4012888888881881</t>
+  </si>
+  <si>
+    <t>visa</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>US/CA (+1)</t>
+  </si>
+  <si>
+    <t>6280888815760052</t>
+  </si>
+  <si>
+    <t>CreditCard</t>
+  </si>
+  <si>
+    <t>1234567854</t>
   </si>
   <si>
     <t>TC_11057</t>
   </si>
   <si>
-    <t>TestCaseId</t>
-  </si>
-  <si>
-    <t>PaymentMethod</t>
-  </si>
-  <si>
-    <t>MerchantName</t>
-  </si>
-  <si>
-    <t>VaultCustomerName</t>
-  </si>
-  <si>
-    <t>TotalAmount</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>PaymentType</t>
-  </si>
-  <si>
-    <t>CardNumber</t>
-  </si>
-  <si>
-    <t>CardExpiry</t>
-  </si>
-  <si>
-    <t>CardType</t>
-  </si>
-  <si>
-    <t>QuickSaleItemName</t>
-  </si>
-  <si>
-    <t>QuickSaleItemPrice</t>
-  </si>
-  <si>
-    <t>QuickSaleItemTax</t>
-  </si>
-  <si>
-    <t>PresetSaleItem</t>
-  </si>
-  <si>
-    <t>CustomerAddress</t>
-  </si>
-  <si>
-    <t>CustomerState</t>
-  </si>
-  <si>
-    <t>CustomerCity</t>
-  </si>
-  <si>
-    <t>CustomerZipCode</t>
-  </si>
-  <si>
-    <t>CustomerCountry</t>
-  </si>
-  <si>
-    <t>CountryCode</t>
-  </si>
-  <si>
-    <t>OrderNote</t>
-  </si>
-  <si>
-    <t>DiscountRate</t>
-  </si>
-  <si>
-    <t>TaxAmount</t>
-  </si>
-  <si>
-    <t>Discount</t>
-  </si>
-  <si>
-    <t>PhoneCode</t>
-  </si>
-  <si>
-    <t>MID</t>
-  </si>
-  <si>
-    <t>TransactionCardType</t>
-  </si>
-  <si>
-    <t>FaxNumber</t>
-  </si>
-  <si>
-    <t>TC_11001</t>
-  </si>
-  <si>
-    <t>Sale</t>
-  </si>
-  <si>
-    <t>QA Fee Test</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>Card</t>
-  </si>
-  <si>
-    <t>5555555555554444</t>
-  </si>
-  <si>
-    <t>mastercard</t>
-  </si>
-  <si>
-    <t>Banana</t>
-  </si>
-  <si>
-    <t>No Tax</t>
-  </si>
-  <si>
-    <t>Apple</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>Buy Fruits</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>TC_11055</t>
-  </si>
-  <si>
-    <t>Refund</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>4012888888881881</t>
-  </si>
-  <si>
-    <t>visa</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>US/CA (+1)</t>
-  </si>
-  <si>
-    <t>6280888815760052</t>
-  </si>
-  <si>
-    <t>CreditCard</t>
-  </si>
-  <si>
-    <t>1234567854</t>
-  </si>
-  <si>
     <t>TC_11059</t>
   </si>
   <si>
@@ -384,55 +429,106 @@
     <t/>
   </si>
   <si>
+    <t>987654321</t>
+  </si>
+  <si>
+    <t>Checking</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>10167</t>
+  </si>
+  <si>
+    <t>CreatePaymentMethod</t>
+  </si>
+  <si>
+    <t>6CA98F60-0828-4F7F-A692-75A71719BCBE</t>
+  </si>
+  <si>
+    <t>4007702835532454</t>
+  </si>
+  <si>
+    <t>11985</t>
+  </si>
+  <si>
+    <t>AutomationChange</t>
+  </si>
+  <si>
+    <t>4001919257537193</t>
+  </si>
+  <si>
+    <t>CreatePaymentSubscriptionACH</t>
+  </si>
+  <si>
     <t>026009593</t>
   </si>
   <si>
-    <t>Checking</t>
-  </si>
-  <si>
-    <t>987654321</t>
-  </si>
-  <si>
-    <t>CreatePaymentMethod</t>
-  </si>
-  <si>
-    <t>6CA98F60-0828-4F7F-A692-75A71719BCBE</t>
-  </si>
-  <si>
-    <t>4007702835532454</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>11985</t>
-  </si>
-  <si>
-    <t>AutomationChange</t>
-  </si>
-  <si>
-    <t>4001919257537193</t>
-  </si>
-  <si>
-    <t>Test execution for CreatePayment_Card started 03/28/2024 20:50:22</t>
-  </si>
-  <si>
-    <t>Test execution for CreatePayment_Card ended 03/28/2024 20:50:38</t>
-  </si>
-  <si>
-    <t>Test execution for CreatePayment_Token started 03/28/2024 20:50:39</t>
-  </si>
-  <si>
-    <t>Test execution for CreatePayment_Token ended 03/28/2024 20:50:50</t>
+    <t>111000025</t>
   </si>
   <si>
     <t>Flag status - disabled</t>
   </si>
   <si>
-    <t>Test execution for CreateSubscription_Card started 03/28/2024 20:50:50</t>
-  </si>
-  <si>
-    <t>Test execution for CreateSubscription_Card ended 03/28/2024 20:51:08</t>
+    <t>Test execution for TC_11067 and TC_11068 started 04/08/2024 18:54:24</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11067 and TC_11068 ended 04/08/2024 19:00:28</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11069 and TC_11070 started 04/08/2024 19:00:28</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11069 and TC_11070 ended 04/08/2024 19:06:27</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11071 and TC_11072 started 04/08/2024 19:06:27</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11071 and TC_11072 ended 04/08/2024 19:12:24</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11073 and TC_11074 started 04/08/2024 19:12:24</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11073 and TC_11074 ended 04/08/2024 19:18:22</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11075 and TC_11076 started 04/08/2024 19:18:22</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11075 and TC_11076 ended 04/08/2024 19:24:25</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11055 and TC_11056 started 04/08/2024 19:24:25</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11055 and TC_11056 ended 04/08/2024 19:29:33</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11057 and TC_11058 started 04/08/2024 19:29:33</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11057 and TC_11058 ended 04/08/2024 19:34:46</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11059 and TC_11060 started 04/08/2024 19:34:46</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11059 and TC_11060 ended 04/08/2024 19:40:27</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11061 and TC_11062 started 04/08/2024 19:40:27</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11061 and TC_11062 ended 04/08/2024 19:45:27</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11063 and TC_11064 started 04/08/2024 19:45:27</t>
+  </si>
+  <si>
+    <t>Test execution for TC_11063 and TC_11064 ended 04/08/2024 19:50:40</t>
   </si>
   <si>
     <t>PaymentsNewCustomer</t>
@@ -480,10 +576,7 @@
     <t>TC_11009 and TC_11010</t>
   </si>
   <si>
-    <t>111000025</t>
-  </si>
-  <si>
-    <t>10167</t>
+    <t>2CB4CF34-8FC4-4A0C-AEDC-78B39D168587</t>
   </si>
 </sst>
 </file>
@@ -873,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -927,18 +1020,18 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -949,7 +1042,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -960,13 +1053,145 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -982,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,615 +1232,615 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="J1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="K1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="L1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="M1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="N1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="O1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="P1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="Q1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="R1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="S1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="T1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="U1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="V1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="W1" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="X1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="Y1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="Z1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="AA1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="AB1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="AC1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="AD1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="AE1" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="I2">
         <v>1231233332</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="L2">
         <v>1030</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="N2" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="O2">
         <v>20</v>
       </c>
       <c r="P2" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="Q2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="R2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="S2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="T2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="U2">
         <v>12343</v>
       </c>
       <c r="V2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="W2" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="X2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="Y2" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
         <v>67</v>
-      </c>
-      <c r="C3" t="s">
-        <v>53</v>
       </c>
       <c r="E3">
         <v>50</v>
       </c>
       <c r="F3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="I3">
         <v>1231233332</v>
       </c>
       <c r="J3" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="L3">
         <v>1030</v>
       </c>
       <c r="M3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="R3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="S3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="T3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="U3">
         <v>12343</v>
       </c>
       <c r="V3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="W3" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="X3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AB3" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="AD3" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
         <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
       </c>
       <c r="E4">
         <v>50</v>
       </c>
       <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="I4">
         <v>1231233332</v>
       </c>
       <c r="J4" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="L4">
         <v>1030</v>
       </c>
       <c r="M4" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="R4" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="S4" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="T4" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="U4">
         <v>12343</v>
       </c>
       <c r="V4" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="W4" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="X4" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AB4" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="AD4" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
       </c>
       <c r="E5">
         <v>50</v>
       </c>
       <c r="F5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="I5">
         <v>1231233332</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="L5">
         <v>1030</v>
       </c>
       <c r="M5" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="R5" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="S5" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="T5" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="U5">
         <v>12343</v>
       </c>
       <c r="V5" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="W5" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="X5" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AB5" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="AD5" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
         <v>67</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
       </c>
       <c r="E6">
         <v>50</v>
       </c>
       <c r="F6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="I6">
         <v>1231233332</v>
       </c>
       <c r="J6" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="L6">
         <v>1030</v>
       </c>
       <c r="M6" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="R6" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="S6" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="T6" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="U6">
         <v>12343</v>
       </c>
       <c r="V6" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="W6" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="X6" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AB6" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="AD6" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
         <v>67</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
       </c>
       <c r="E7">
         <v>50</v>
       </c>
       <c r="F7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="I7">
         <v>1231233332</v>
       </c>
       <c r="J7" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="L7">
         <v>1030</v>
       </c>
       <c r="M7" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="R7" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="S7" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="T7" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="U7">
         <v>12343</v>
       </c>
       <c r="V7" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="W7" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="X7" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AB7" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="AD7" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
         <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
       </c>
       <c r="E8">
         <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="I8">
         <v>1231233332</v>
       </c>
       <c r="J8" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="L8">
         <v>1030</v>
       </c>
       <c r="M8" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="R8" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="S8" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="T8" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="U8">
         <v>12343</v>
       </c>
       <c r="V8" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="W8" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="X8" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1638,10 +1863,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1653,316 +1878,393 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="J1" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="K1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="L1" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="M1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="N1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="O1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="P1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="Q1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="R1" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="S1" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="T1" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="U1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="V1" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="W1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="X1" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="Y1" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="Z1" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="AA1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="AB1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
         <v>68</v>
       </c>
-      <c r="F2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" t="s">
-        <v>54</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="N2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="O2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="R2" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="Z2" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="AA2" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" t="s">
         <v>68</v>
       </c>
-      <c r="F3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="M3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="N3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="O3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="Q3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="R3" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="T3" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="Z3" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="AA3" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="I4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" t="s">
+        <v>75</v>
+      </c>
+      <c r="O4" t="s">
+        <v>75</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>76</v>
+      </c>
+      <c r="R4" t="s">
+        <v>77</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="T4" t="s">
+        <v>134</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="X4" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" t="s">
         <v>68</v>
       </c>
-      <c r="F4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="M4" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4" t="s">
-        <v>61</v>
-      </c>
-      <c r="O4" t="s">
-        <v>61</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>62</v>
-      </c>
-      <c r="R4" t="s">
-        <v>63</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="T4" t="s">
-        <v>119</v>
-      </c>
-      <c r="U4" s="2" t="s">
+      <c r="L5" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="X4" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Q5" t="s">
+        <v>76</v>
+      </c>
+      <c r="R5" t="s">
+        <v>77</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="T5" t="s">
+        <v>134</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z5" t="s">
         <v>127</v>
       </c>
-      <c r="Z4" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>114</v>
+      <c r="AA5" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1976,7 +2278,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2016,10 +2318,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -2033,32 +2335,32 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -2067,15 +2369,15 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -2084,27 +2386,231 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" t="s">
-        <v>132</v>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2149,79 +2655,79 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>